<commit_message>
caso de uso 003 boceto a duda final 1
</commit_message>
<xml_diff>
--- a/CU_003_Regist_NFC.xlsx
+++ b/CU_003_Regist_NFC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juab\Desktop\ProyectoFinalAnalisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F94D4414-BF72-4466-BDA2-9E291EDBE881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746585FC-AF51-41CC-8B73-789CD7CDBBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,106 +28,7 @@
         <rFont val="Calibri"/>
         <family val="1"/>
       </rPr>
-      <t>ID:    CU_001</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Usuario del Sistema: Valida los RFC para asegurarse de que correspondan a contribuyentes registrados en el SAT. Administrador del Sistema: Garantizar el correcto funcionamiento y seguridad del sistema.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Servicio de Administración Tributaria (SAT): Asegurar que solo se acceda a información autorizada. Desarrollador del Sistema: Asegurar que el sistema funcione correctamente y se mantenga actualizado.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Este caso de uso describe el proceso de validación de un Registro Federal de Contribuyentes (RFC) utilizando la lista de contribuyentes del Servicio de Administración Tributaria (SAT) como fuente de datos.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>El usuario inicia el proceso de validación al solicitar la verificación de un RFC.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Evento</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Nombre del caso de uso: Validar RFC con Lista del SAT</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Nivel de importancia: Alta</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Actor principal: Usuario del sistema</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
       <t>Tipo de caso de uso: funcional</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Partes interesadas e intereses:</t>
     </r>
   </si>
   <si>
@@ -161,155 +62,67 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Relaciones:
+    <t>ID:    CU_003</t>
+  </si>
+  <si>
+    <t>Nombre del caso de uso: Sistema Asistemcia  tarjetas metro, lectura NFC.</t>
+  </si>
+  <si>
+    <t>Nivel de importancia: Alta</t>
+  </si>
+  <si>
+    <t>Relaciones:
+Asociación:                              Incluisión:                                    Extensión:                       Generalización:</t>
+  </si>
+  <si>
+    <t>Actor principal: Profesor</t>
+  </si>
+  <si>
+    <t>Partes interesadas e intereses:</t>
+  </si>
+  <si>
+    <t>Profesor:
+Registrar la asistencia de los alumnos de manera eficiente y precisa.
+Tener acceso a un sistema fácil de usar que no requiera una curva de aprendizaje prolongada.
+Contar con un registro de asistencia actualizado en tiempo real.
+Alumno:
+Facilitar el proceso de registro de asistencia.
+Asegurarse de que su asistencia quede registrada correctamente.
+Evitar la pérdida de tiempo en el proceso de registro.</t>
+  </si>
+  <si>
+    <t>Flujo normal de eventos:
+1. El profesor selecciona la opción de "Registro de Asistencia con Tarjetas NFC" desde el menú principal.
+2.  El sistema activa la lectura NFC y espera a que se acerque una tarjeta válida.
+4. El alumno presenta su tarjeta del metro con tecnología NFC al lector del sistema.
+5. El sistema verifica la validez de la tarjeta y registra la asistencia del alumno asociado a esa tarjeta.
+6. El sistema actualiza el registro de asistencia en tiempo real.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subflujos:
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Asociación: Incluisión: Extensión: Generalización:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Flujo normal de eventos:
+  </si>
+  <si>
+    <t>Este caso de uso describe el proceso mediante el cual un profesor registra la asistencia de un alumno utilizando una tarjeta del metro de la Ciudad de México con tecnología NFC.</t>
+  </si>
+  <si>
+    <t>Este caso de uso es desencadenado cuando el profesor selecciona la opción de "Registro de Asistencia con Tarjetas NFC" desde el menú principal del sistema.</t>
+  </si>
+  <si>
+    <t>Interacción del usuario con el sistema.</t>
+  </si>
+  <si>
+    <t>Este caso de uso está asociado con el sistema de asistencia para profesores de la FCA y se relaciona específicamente con el registro de asistencia a través de tarjetas NFC del metro de la CDMX.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flujos alternativos/excepciones:
+FA_1: Tarjeta Inválida:
+Si la tarjeta no es válida, el sistema muestra un mensaje de error y vuelve al paso 2 del flujo normal de eventos.
+EX_1: Fallo en la Lectura NFC:
+Si hay un fallo en la lectura NFC, el sistema muestra un mensaje de error y vuelve al paso 2 del flujo normal de eventos.
+EX_2: Conexión a Internet Perdida:
+Si se pierde la conexión a Internet durante el proceso de registro, el sistema muestra un mensaje de error y vuelve al paso 2 del flujo normal de eventos.
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">El caso de uso comienza cuando el usuario solicita la validación de un RFC. El sistema solicita al usuario que ingrese el RFC que desea validar.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">El usuario ingresa el RFC a ser validado.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">El sistema verifica que el RFC ingresado tenga el formato correcto. Si el formato es incorrecto, se muestra un mensaje de error y se regresa al paso 2.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">El sistema consulta la lista de contribuyentes del SAT para verificar si el RFC proporcionado está presente.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Si el RFC se encuentra en la lista, el sistema confirma que el RFC es válido y proporciona la información asociada al contribuyente (nombre, dirección, etc.).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Si el RFC no se encuentra en la lista, el sistema indica que el RFC no es válido y proporciona un mensaje de error.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Suflujos:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">S-1: Conexión con la Base de Datos del SAT
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">1.El sistema intenta conectar con la base de datos del SAT.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.Si hay un fallo en la conexión, se muestra un mensaje de error y se sugiere intentarlo más tarde. Subflujo 2: RFC no encontrado en la lista
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1.Si el RFC no se encuentra en la lista de contribuyentes, se muestra un mensaje indicando que el RFC no es válido.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Flujos alternativos/excepciones:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>4a: Si el formato del RFC es incorrecto, el sistema muestra un mensaje de error y solicita al usuario que ingrese un RFC válido.</t>
-    </r>
-  </si>
-  <si>
-    <t>SAT y Usuario del Sistema</t>
   </si>
 </sst>
 </file>
@@ -480,22 +293,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -516,47 +353,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,10 +675,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D3"/>
+      <selection activeCell="A11" sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75"/>
@@ -876,107 +692,107 @@
     <col min="4" max="4" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:4" ht="27.75" customHeight="1">
+      <c r="A1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A2" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" ht="105.75" customHeight="1">
+      <c r="A4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" ht="57.6" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" ht="45.95" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="1:4" ht="38.85" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8" spans="1:4" ht="81.75" customHeight="1">
+      <c r="A8" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="26"/>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="1:4" ht="54.2" customHeight="1">
-      <c r="A4" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="1:4" ht="57.6" customHeight="1">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-    </row>
-    <row r="6" spans="1:4" ht="45.95" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="B8" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:4" ht="93.75" customHeight="1">
+      <c r="A9" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-    </row>
-    <row r="7" spans="1:4" ht="38.85" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:4" ht="24" customHeight="1">
+      <c r="A10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="8" spans="1:4" ht="74.099999999999994" customHeight="1">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:4" ht="140.25" customHeight="1">
+      <c r="A11" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" ht="187.35" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" ht="119.45" customHeight="1">
-      <c r="A10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" ht="57.6" customHeight="1">
-      <c r="A11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:4" ht="16.5" customHeight="1"/>
     <row r="13" spans="1:4" ht="16.5" customHeight="1"/>
@@ -1002,6 +818,11 @@
     <row r="33" ht="57.6" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="B5:D5"/>
@@ -1009,12 +830,8 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="98" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>